<commit_message>
run with 30 sep 2020 data
</commit_message>
<xml_diff>
--- a/EFI/CODE/input/bmk.xlsx
+++ b/EFI/CODE/input/bmk.xlsx
@@ -56,10 +56,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -147,7 +148,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -161,6 +162,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Migliaia 2" xfId="2"/>
@@ -477,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E186"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="B188" sqref="B188"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -490,7 +492,8 @@
     <col min="3" max="3" width="34.7109375" style="12" customWidth="1"/>
     <col min="4" max="4" width="23.140625" style="12" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" style="12" customWidth="1"/>
-    <col min="6" max="158" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="158" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="159" max="159" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="160" max="161" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="162" max="16384" width="9.140625" style="12"/>
@@ -3485,7 +3488,7 @@
         <v>3.6968000000000001E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>20191031</v>
       </c>
@@ -3502,7 +3505,7 @@
         <v>1.0428999999999999E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>20191129</v>
       </c>
@@ -3519,7 +3522,7 @@
         <v>2.8284000000000004E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>20191231</v>
       </c>
@@ -3536,7 +3539,7 @@
         <v>2.1337999999999999E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>20200131</v>
       </c>
@@ -3553,7 +3556,7 @@
         <v>-1.1766E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>20200228</v>
       </c>
@@ -3570,7 +3573,7 @@
         <v>-8.340199999999999E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>20200331</v>
       </c>
@@ -3587,7 +3590,7 @@
         <v>-0.14513999999999999</v>
       </c>
     </row>
-    <row r="183" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>20200430</v>
       </c>
@@ -3604,7 +3607,7 @@
         <v>6.5012E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>20200529</v>
       </c>
@@ -3621,7 +3624,7 @@
         <v>3.4047999999999995E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>20200630</v>
       </c>
@@ -3638,22 +3641,58 @@
         <v>3.0561999999999999E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>20200731</v>
       </c>
       <c r="B186" s="9">
-        <v>1.361812113623031</v>
+        <v>1.3766637156608588</v>
       </c>
       <c r="C186" s="2">
         <v>-9.0959999999999999E-3</v>
       </c>
-      <c r="D186" s="9">
+      <c r="D186" s="10">
         <v>1.1445696414863842</v>
       </c>
       <c r="E186" s="3">
         <v>-9.5340000000000008E-3</v>
       </c>
+    </row>
+    <row r="187" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="4">
+        <v>20200831</v>
+      </c>
+      <c r="B187" s="9">
+        <v>1.4498221781563312</v>
+      </c>
+      <c r="C187" s="2">
+        <v>3.0781999999999997E-2</v>
+      </c>
+      <c r="D187" s="10">
+        <v>1.2100712320463027</v>
+      </c>
+      <c r="E187" s="3">
+        <v>3.0543000000000001E-2</v>
+      </c>
+      <c r="F187" s="13"/>
+    </row>
+    <row r="188" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="4">
+        <v>20200930</v>
+      </c>
+      <c r="B188" s="9">
+        <v>1.4158014975682742</v>
+      </c>
+      <c r="C188" s="2">
+        <v>-1.3887E-2</v>
+      </c>
+      <c r="D188" s="10">
+        <v>1.1789954204524995</v>
+      </c>
+      <c r="E188" s="3">
+        <v>-1.4060999999999999E-2</v>
+      </c>
+      <c r="F188" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes to FMP to use US data. TO DO: rewrite input section
</commit_message>
<xml_diff>
--- a/EFI/CODE/input/bmk.xlsx
+++ b/EFI/CODE/input/bmk.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u369343\Desktop\EFI\CODE\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\u093799\Documents\GitHub\PrimoRepository\EFI\CODE\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3200C30F-47BA-48D0-A14A-DE72907788E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BMK" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,6 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -55,12 +59,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -146,7 +150,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -158,14 +162,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Migliaia 2" xfId="2"/>
+    <cellStyle name="Migliaia 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -478,11 +482,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F188"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="G4:H4"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3694,6 +3698,23 @@
       </c>
       <c r="F188" s="13"/>
     </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="4">
+        <v>20201030</v>
+      </c>
+      <c r="B189" s="9">
+        <v>1.4158014975682742</v>
+      </c>
+      <c r="C189" s="2">
+        <v>-1.3887E-2</v>
+      </c>
+      <c r="D189" s="10">
+        <v>1.1789954204524995</v>
+      </c>
+      <c r="E189" s="3">
+        <v>-1.4060999999999999E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new data & small changes to becktestMAIN and readBMK to deal with empty bmk cells and to delete output file before writing new data
</commit_message>
<xml_diff>
--- a/EFI/CODE/input/bmk.xlsx
+++ b/EFI/CODE/input/bmk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\u093799\Documents\GitHub\PrimoRepository\EFI\CODE\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u369343\Desktop\EFI\CODE\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3200C30F-47BA-48D0-A14A-DE72907788E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE340FC-347D-489B-AC05-1B98401F5E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BMK" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -167,6 +167,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Migliaia 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -483,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F189"/>
+  <dimension ref="A1:F190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="C195" sqref="C195"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="H179" sqref="H179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3698,22 +3699,26 @@
       </c>
       <c r="F188" s="13"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>20201030</v>
       </c>
       <c r="B189" s="9">
-        <v>1.4158014975682742</v>
+        <v>1.2928734383645129</v>
       </c>
       <c r="C189" s="2">
-        <v>-1.3887E-2</v>
+        <v>-5.0885E-2</v>
       </c>
       <c r="D189" s="10">
-        <v>1.1789954204524995</v>
+        <v>1.0677315562933538</v>
       </c>
       <c r="E189" s="3">
-        <v>-1.4060999999999999E-2</v>
-      </c>
+        <v>-5.1062000000000003E-2</v>
+      </c>
+      <c r="F189" s="13"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C190" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>